<commit_message>
First commit of CMIP5 -> CMIP6 mapping for ocean realm
</commit_message>
<xml_diff>
--- a/mappings/cmip5-ocean-key-properties.xlsx
+++ b/mappings/cmip5-ocean-key-properties.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
-  <workbookPr date1904="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/esdoc-docs/cmip5/vocab-mappings/ocean/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26819"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15500" windowHeight="17480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>Table 1</t>
   </si>
@@ -147,13 +142,49 @@
   </si>
   <si>
     <t>cmip6-id</t>
+  </si>
+  <si>
+    <t>Ocean &gt; Key Properties &gt; Bathymetry &gt; Bathymetry Reference Dates</t>
+  </si>
+  <si>
+    <t>Ocean &gt; Key Properties &gt; Bathymetry &gt; Ocean Bathymetry Type</t>
+  </si>
+  <si>
+    <t>Ocean &gt; Grid &gt; Discretisation &gt; Horizontal &gt; Pole Singularity Treatment</t>
+  </si>
+  <si>
+    <t>Ocean &gt; Key Properties &gt; General &gt; Basic Approximations</t>
+  </si>
+  <si>
+    <t>Ocean &gt; Grid &gt; Discretisation &gt; Horizontal &gt; Scheme</t>
+  </si>
+  <si>
+    <t>Ocean &gt; Grid &gt; Horizontal Grid &gt; Horizontal Grid Type</t>
+  </si>
+  <si>
+    <t>Ocean &gt; Key Properties &gt; General &gt; Prognostic Variables</t>
+  </si>
+  <si>
+    <t>Ocean &gt; Key Properties &gt; General &gt; Model Family</t>
+  </si>
+  <si>
+    <t>Ocean &gt; Key Properties &gt; Seawater Properties &gt; Seawater Eos Type</t>
+  </si>
+  <si>
+    <t>Ocean &gt; Key Properties &gt; Seawater Properties &gt; Ocean Freezing Point</t>
+  </si>
+  <si>
+    <t>Ocean &gt; Key Properties &gt; Seawater Properties &gt; Ocean Specific Heat</t>
+  </si>
+  <si>
+    <t>Ocean &gt; Timestepping Framework &gt; Timestepping Attributes &gt; Time Step</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -169,6 +200,11 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -244,7 +280,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -274,6 +310,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1467,19 +1506,19 @@
   <dimension ref="A1:IV44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="58" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="43" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" style="1" customWidth="1"/>
     <col min="5" max="256" width="8.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="28" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1487,7 +1526,7 @@
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="20.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1501,133 +1540,149 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="20.5" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="D3" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="20.25" customHeight="1">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="20.25" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="D5" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="20.25" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="D6" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="20.25" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="20.25" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="D8" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="20.25" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="D9" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="20.25" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="D10" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="20.25" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="20.25" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="D12" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="20.25" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="20.25" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="D14" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="20.25" customHeight="1">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="20.25" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
@@ -1639,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="20.25" customHeight="1">
       <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
@@ -1651,13 +1706,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="20.25" customHeight="1">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="20.25" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>4</v>
       </c>
@@ -1669,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="20.25" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>4</v>
       </c>
@@ -1681,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="20.25" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>4</v>
       </c>
@@ -1693,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="20.25" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
@@ -1705,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="20.25" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
@@ -1717,7 +1772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="20.25" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>4</v>
       </c>
@@ -1729,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="20.25" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>4</v>
       </c>
@@ -1741,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="20.25" customHeight="1">
       <c r="A26" s="6" t="s">
         <v>4</v>
       </c>
@@ -1753,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="20.25" customHeight="1">
       <c r="A27" s="6" t="s">
         <v>4</v>
       </c>
@@ -1765,7 +1820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="20.25" customHeight="1">
       <c r="A28" s="6" t="s">
         <v>4</v>
       </c>
@@ -1777,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="20.25" customHeight="1">
       <c r="A29" s="6" t="s">
         <v>4</v>
       </c>
@@ -1789,7 +1844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="20.25" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>4</v>
       </c>
@@ -1801,7 +1856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="20.25" customHeight="1">
       <c r="A31" s="6" t="s">
         <v>4</v>
       </c>
@@ -1813,7 +1868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="20.25" customHeight="1">
       <c r="A32" s="6" t="s">
         <v>4</v>
       </c>
@@ -1825,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="20.25" customHeight="1">
       <c r="A33" s="6" t="s">
         <v>4</v>
       </c>
@@ -1837,37 +1892,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="20.25" customHeight="1">
       <c r="A34" s="6"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="20.25" customHeight="1">
       <c r="A35" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="7"/>
+      <c r="C35" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="D35" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="20.25" customHeight="1">
       <c r="A36" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="7"/>
+      <c r="C36" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="D36" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="20.25" customHeight="1">
       <c r="A37" s="6" t="s">
         <v>4</v>
       </c>
@@ -1879,19 +1938,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="20.25" customHeight="1">
       <c r="A38" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="10" t="s">
+        <v>50</v>
+      </c>
       <c r="D38" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="20.25" customHeight="1">
       <c r="A39" s="6" t="s">
         <v>4</v>
       </c>
@@ -1903,13 +1964,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="20.25" customHeight="1">
       <c r="A40" s="6"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="20.25" customHeight="1">
       <c r="A41" s="6" t="s">
         <v>4</v>
       </c>
@@ -1921,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="20.25" customHeight="1">
       <c r="A42" s="6" t="s">
         <v>4</v>
       </c>
@@ -1933,19 +1994,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="20.25" customHeight="1">
       <c r="A43" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="7"/>
+      <c r="C43" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="D43" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4" ht="20.25" customHeight="1">
       <c r="A44" s="6" t="s">
         <v>4</v>
       </c>
@@ -1966,5 +2029,10 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mapping files updated in readiness for new job to automatically seed CMIP^ documents from CMIP5
</commit_message>
<xml_diff>
--- a/mappings/cmip5-ocean-key-properties.xlsx
+++ b/mappings/cmip5-ocean-key-properties.xlsx
@@ -1,42 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26819"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/cmip6-specializations-ocean/mappings/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15500" windowHeight="17480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24420" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
-  <si>
-    <t>Table 1</t>
-  </si>
-  <si>
-    <t>cmip5-property-type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>cmip5-component-property</t>
-  </si>
-  <si>
-    <t>mapping-qc-status</t>
-  </si>
-  <si>
-    <t>Key Properties</t>
   </si>
   <si>
     <t>Basic Approximations</t>
@@ -280,7 +273,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -290,29 +283,17 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1503,536 +1484,299 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV44"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="1" customWidth="1"/>
-    <col min="5" max="256" width="8.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43" style="1" customWidth="1"/>
+    <col min="2" max="2" width="61" style="1" customWidth="1"/>
+    <col min="3" max="254" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28" customHeight="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-    </row>
-    <row r="2" spans="1:4" ht="20.5" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="20.5" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="B6" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B8" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="B9" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="7" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="4"/>
+    </row>
+    <row r="30" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="4"/>
+    </row>
+    <row r="31" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="4"/>
+    </row>
+    <row r="32" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="4"/>
+    </row>
+    <row r="33" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="10" t="s">
+    </row>
+    <row r="36" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="10" t="s">
+    </row>
+    <row r="37" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="4"/>
+    </row>
+    <row r="38" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="10" t="s">
+    </row>
+    <row r="39" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="4"/>
+    </row>
+    <row r="40" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+    </row>
+    <row r="41" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="4"/>
+    </row>
+    <row r="42" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="4"/>
+    </row>
+    <row r="43" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A16" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A19" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A21" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A22" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A23" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A27" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A29" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A30" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A31" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A32" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A34" s="6"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="8"/>
-    </row>
-    <row r="35" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A35" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A36" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A37" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A38" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A39" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="7" t="s">
+    </row>
+    <row r="44" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A40" s="6"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="8"/>
-    </row>
-    <row r="41" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A41" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A42" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A43" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D43" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A44" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="8">
-        <v>0</v>
-      </c>
+      <c r="B44" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>